<commit_message>
Continuing to prepare Christian's samples for processing. Added in the metadata to all the pH files and sorted the data in order they were ran.
Created the metadata file for each alkalinity run.
</commit_message>
<xml_diff>
--- a/check sample work/christains samples 2021/TA/2021-04-28-run/20210428 pH electrode check sheet.xlsx
+++ b/check sample work/christains samples 2021/TA/2021-04-28-run/20210428 pH electrode check sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lab\Desktop\carbon chemistry benchtop comp\pH electrode checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\christains samples 2021\TA\2021-04-28-run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875617A7-447D-47F6-92CF-1BA4376D87AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48060470-7A8D-4750-80A3-73FD8208E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="1740" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pH to mV from calibration" sheetId="4" r:id="rId1"/>
@@ -20,14 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -614,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1226,7 +1218,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,7 +1491,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>49.898000000000003</v>

</xml_diff>